<commit_message>
promo review fall 2021
</commit_message>
<xml_diff>
--- a/data/appointment.xlsx
+++ b/data/appointment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjysk\Box Sync\JY\blogging\cover_letter\CV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00315273\Documents\GitHub\jy_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF72185A-C0D5-4213-869C-B96B546A3A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78400E8E-5E77-4CFA-9C27-4272621216DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>what</t>
   </si>
@@ -42,22 +42,90 @@
     <t>why</t>
   </si>
   <si>
-    <t>Assistant Professor</t>
-  </si>
-  <si>
-    <t>School of Information Sciences</t>
-  </si>
-  <si>
-    <t>University of Illinois at Urbana-Champaign</t>
-  </si>
-  <si>
-    <t>Sep. 2021</t>
-  </si>
-  <si>
-    <t>Faculty Affiliate</t>
-  </si>
-  <si>
-    <t>Illinois Informatics Institute</t>
+    <t>Assistant Research Professor</t>
+  </si>
+  <si>
+    <t>2015-present</t>
+  </si>
+  <si>
+    <t>Psychology Department, College of Education and Human Services</t>
+  </si>
+  <si>
+    <t>Utah State University</t>
+  </si>
+  <si>
+    <t>Director, The Statistical Consulting Studio</t>
+  </si>
+  <si>
+    <t>Instructor, graduate student quantitatice methods and statistics courses</t>
+  </si>
+  <si>
+    <t>Statistician</t>
+  </si>
+  <si>
+    <t>2013-2015</t>
+  </si>
+  <si>
+    <t>Office of Research Services, College of Education and Human Services</t>
+  </si>
+  <si>
+    <t>Acting Director, Office of Methodological and Data Sciences</t>
+  </si>
+  <si>
+    <t>Statistician and Data Manager</t>
+  </si>
+  <si>
+    <t>2005-2013</t>
+  </si>
+  <si>
+    <t>Center for Epidemiology</t>
+  </si>
+  <si>
+    <t>Managed databases, clean data, and prepare custom datasets</t>
+  </si>
+  <si>
+    <t>Performed statistical analyses and prepared publications, posters, presentations,
+and grant submissions</t>
+  </si>
+  <si>
+    <t>Worked under three main grants and many co-investigators: University of Utah,
+  BYU, Duke, John Hopkins, University of Maryland, ect.</t>
+  </si>
+  <si>
+    <t>Data Manager</t>
+  </si>
+  <si>
+    <t>Kenoi Genetics Lab</t>
+  </si>
+  <si>
+    <t>Brigham Young University</t>
+  </si>
+  <si>
+    <t>Managed databases and prepare custom datasets</t>
+  </si>
+  <si>
+    <t>Adjunct Lecturer</t>
+  </si>
+  <si>
+    <t>2006-2008</t>
+  </si>
+  <si>
+    <t>Mathematics and Statistics Department</t>
+  </si>
+  <si>
+    <t>Traditional, evening, and distance courses</t>
+  </si>
+  <si>
+    <t>High School Teacher, Math and Science</t>
+  </si>
+  <si>
+    <t>2000-2004</t>
+  </si>
+  <si>
+    <t>Sky View High School, Smithfield, Utah</t>
+  </si>
+  <si>
+    <t>Logan River Academy, Logan, Utah</t>
   </si>
 </sst>
 </file>
@@ -95,7 +163,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,15 +446,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="53.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,32 +474,179 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>2012</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>